<commit_message>
20210617 CRE20-006	Interface with eHRSS to support payment settlement by healhcare voucher in DHC 20210617 CRE20-021	To allow EHCP to choose make claims for respective District Health Centres (DHCs) and to generate reports and statistics for respective DHCs
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSM0005-SP_Data_File_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSM0005-SP_Data_File_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2019\CRE16-022 (SDIR Remark)\Front-end\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-006 (DHC Integration)\Front-end\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="19230" windowHeight="6060" tabRatio="679"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19230" windowHeight="6060" tabRatio="679" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="102">
   <si>
     <t>Sub Report ID</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -352,6 +352,18 @@
   </si>
   <si>
     <t xml:space="preserve">To add a new optional field “Remarks” in the eHS(S) </t>
+  </si>
+  <si>
+    <t>Enrolled DHC (Any Practice)</t>
+  </si>
+  <si>
+    <t>Enrolled DHC</t>
+  </si>
+  <si>
+    <t>CRE20-006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To modify Report eHS(S)M0005 by adding Enrolled DHC column </t>
   </si>
 </sst>
 </file>
@@ -359,13 +371,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="1"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -502,16 +514,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1">
@@ -547,7 +559,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -946,15 +958,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="1" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
+    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -962,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>29</v>
       </c>
@@ -970,7 +982,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15">
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="33" t="s">
         <v>31</v>
       </c>
@@ -978,7 +990,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15">
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="33" t="s">
         <v>33</v>
       </c>
@@ -986,7 +998,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>35</v>
       </c>
@@ -994,10 +1006,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15">
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6"/>
     </row>
-    <row r="7" spans="1:2" ht="15.75">
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>7</v>
       </c>
@@ -1013,32 +1025,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" style="28" customWidth="1"/>
     <col min="2" max="2" width="75.7109375" style="30" customWidth="1"/>
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="15">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
       <c r="B2" s="29"/>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="27"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="27"/>
     </row>
   </sheetData>
@@ -1050,11 +1062,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="19" customWidth="1"/>
     <col min="2" max="3" width="26.7109375" style="5" customWidth="1"/>
@@ -1073,22 +1085,23 @@
     <col min="18" max="20" width="19.28515625" style="19" customWidth="1"/>
     <col min="21" max="24" width="26.7109375" style="19" customWidth="1"/>
     <col min="25" max="25" width="26.7109375" style="50" customWidth="1"/>
-    <col min="26" max="119" width="16.28515625" style="5" customWidth="1"/>
+    <col min="26" max="26" width="32" style="5" customWidth="1"/>
+    <col min="27" max="119" width="16.28515625" style="5" customWidth="1"/>
     <col min="120" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="15.75">
+    <row r="1" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>37</v>
       </c>
       <c r="D1" s="18"/>
       <c r="Q1" s="19"/>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="D2" s="18"/>
       <c r="Q2" s="19"/>
     </row>
-    <row r="3" spans="1:25" s="31" customFormat="1" ht="66" customHeight="1">
+    <row r="3" spans="1:26" s="31" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="43" t="s">
         <v>51</v>
       </c>
@@ -1163,6 +1176,9 @@
       </c>
       <c r="Y3" s="52" t="s">
         <v>94</v>
+      </c>
+      <c r="Z3" s="31" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1178,7 +1194,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="19" customWidth="1"/>
     <col min="2" max="3" width="26.7109375" style="5" customWidth="1"/>
@@ -1197,16 +1213,16 @@
     <col min="19" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="15.75">
+    <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="18"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:18" s="21" customFormat="1" ht="15.75">
+    <row r="3" spans="1:18" s="21" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>8</v>
       </c>
@@ -1274,7 +1290,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="19" customWidth="1"/>
     <col min="2" max="3" width="26.7109375" style="5" customWidth="1"/>
@@ -1296,23 +1312,24 @@
     <col min="25" max="26" width="19.28515625" style="5" customWidth="1"/>
     <col min="27" max="27" width="26.7109375" style="5" customWidth="1"/>
     <col min="28" max="28" width="26.7109375" style="40" customWidth="1"/>
-    <col min="29" max="74" width="22.7109375" style="5" customWidth="1"/>
+    <col min="29" max="29" width="35.7109375" style="5" customWidth="1"/>
+    <col min="30" max="74" width="22.7109375" style="5" customWidth="1"/>
     <col min="75" max="108" width="20.7109375" style="5" customWidth="1"/>
     <col min="109" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="15.75">
+    <row r="1" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="18"/>
       <c r="I1" s="19"/>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="D2" s="18"/>
       <c r="I2" s="19"/>
     </row>
-    <row r="3" spans="1:28" s="31" customFormat="1" ht="63">
+    <row r="3" spans="1:29" s="31" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="48" t="s">
         <v>51</v>
       </c>
@@ -1397,8 +1414,11 @@
       <c r="AB3" s="51" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17" spans="31:31">
+      <c r="AC3" s="31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="31:31" x14ac:dyDescent="0.25">
       <c r="AE17" s="5" t="s">
         <v>24</v>
       </c>
@@ -1416,41 +1436,41 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" style="19" customWidth="1"/>
     <col min="2" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75">
+    <row r="1" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75">
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="15"/>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
     </row>
   </sheetData>
@@ -1465,7 +1485,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" style="5" customWidth="1"/>
     <col min="2" max="2" width="34.7109375" style="5" customWidth="1"/>
@@ -1474,120 +1494,120 @@
     <col min="5" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="10"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="11"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17"/>
       <c r="B4" s="17"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17"/>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="17"/>
       <c r="B7" s="17"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="17"/>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="17"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="17"/>
       <c r="B11" s="17"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="17"/>
       <c r="B12" s="17"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="17"/>
       <c r="B13" s="17"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="17"/>
       <c r="B14" s="17"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="13"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="13"/>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="13"/>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="13"/>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="13"/>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="13"/>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="13"/>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="13"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="13"/>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
       <c r="B26" s="13"/>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
       <c r="B27" s="13"/>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" s="13"/>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
       <c r="B30" s="13"/>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="12"/>
     </row>
   </sheetData>
@@ -1599,11 +1619,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="7" customWidth="1"/>
     <col min="2" max="2" width="18.140625" style="7" bestFit="1" customWidth="1"/>
@@ -1612,13 +1632,13 @@
     <col min="5" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" customHeight="1">
+    <row r="1" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" customHeight="1"/>
-    <row r="3" spans="1:4" s="8" customFormat="1" ht="16.5" customHeight="1">
+    <row r="2" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:4" s="8" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>25</v>
       </c>
@@ -1632,7 +1652,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="40">
         <v>1</v>
       </c>
@@ -1646,7 +1666,7 @@
         <v>41982</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="40">
         <v>2</v>
       </c>
@@ -1660,7 +1680,7 @@
         <v>42255</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="40">
         <v>3</v>
       </c>
@@ -1674,7 +1694,7 @@
         <v>42430</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="40">
         <v>4</v>
       </c>
@@ -1688,7 +1708,7 @@
         <v>42619</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="40">
         <v>5</v>
       </c>
@@ -1702,7 +1722,7 @@
         <v>43340</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="40">
         <v>6</v>
       </c>
@@ -1716,7 +1736,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="40">
         <v>7</v>
       </c>
@@ -1728,6 +1748,20 @@
       </c>
       <c r="D10" s="9">
         <v>43921</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="40">
+        <v>8</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="9">
+        <v>43992</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20210831 CRE21-010-01	To update the requirements due to the introduction of new seasonal influenza vaccines, interval between COVID-19 and other subsidized vaccines and the preparation for the joining of eHRSS under VSS 2021/22
- Phase 1 Enrolment
</commit_message>
<xml_diff>
--- a/EHS2019/EHS/ExcelGenerator/Template/eHSM0005-SP_Data_File_Template.xlsx
+++ b/EHS2019/EHS/ExcelGenerator/Template/eHSM0005-SP_Data_File_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ce5-fs01\ehs$\Development\InternalChangeControl\2020\CRE20-006 (DHC Integration)\Front-end\ExcelGenerator\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub2\EHS\EHS2019\EHS\ExcelGenerator\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="19230" windowHeight="6060" tabRatio="679" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19230" windowHeight="6060" tabRatio="679"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="104">
   <si>
     <t>Sub Report ID</t>
     <phoneticPr fontId="5" type="noConversion"/>
@@ -364,6 +364,14 @@
   </si>
   <si>
     <t xml:space="preserve">To modify Report eHS(S)M0005 by adding Enrolled DHC column </t>
+  </si>
+  <si>
+    <t>CRE21-010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VSS 2021-2022</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -958,7 +966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1025,7 +1033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1314,8 +1322,8 @@
     <col min="28" max="28" width="26.7109375" style="40" customWidth="1"/>
     <col min="29" max="29" width="35.7109375" style="5" customWidth="1"/>
     <col min="30" max="74" width="22.7109375" style="5" customWidth="1"/>
-    <col min="75" max="108" width="20.7109375" style="5" customWidth="1"/>
-    <col min="109" max="16384" width="9.140625" style="5"/>
+    <col min="75" max="115" width="20.7109375" style="5" customWidth="1"/>
+    <col min="116" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
@@ -1619,7 +1627,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1764,6 +1772,20 @@
         <v>43992</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="40">
+        <v>9</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="9">
+        <v>44440</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>